<commit_message>
fix SF max value
</commit_message>
<xml_diff>
--- a/data/vitocal250.xlsx
+++ b/data/vitocal250.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fwu\04_git\bes-rules\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fwu\04_git\heat-pumps-grid-interaction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cop" sheetId="1" r:id="rId1"/>
     <sheet name="cop_extrapolation" sheetId="2" r:id="rId2"/>
     <sheet name="QConMax" sheetId="3" r:id="rId3"/>
+    <sheet name="PEleMax" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,6 +34,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>PeleMax</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,12 +400,12 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:J9"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
@@ -422,7 +437,7 @@
         <v>308.14999999999998</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>293.14999999999998</v>
       </c>
@@ -454,7 +469,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>298.14999999999998</v>
       </c>
@@ -486,7 +501,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>308.14999999999998</v>
       </c>
@@ -518,7 +533,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>318.14999999999998</v>
       </c>
@@ -550,7 +565,7 @@
         <v>7.98</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>328.15</v>
       </c>
@@ -582,7 +597,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>338.15</v>
       </c>
@@ -614,7 +629,7 @@
         <v>4.8499999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>343.15</v>
       </c>
@@ -646,7 +661,7 @@
         <v>4.47</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>363.15</v>
       </c>
@@ -688,12 +703,12 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
@@ -725,7 +740,7 @@
         <v>308.14999999999998</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>308.14999999999998</v>
       </c>
@@ -757,7 +772,7 @@
         <v>8.4017971758664949</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>318.14999999999998</v>
       </c>
@@ -789,7 +804,7 @@
         <v>7.9797979797979801</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>328.15</v>
       </c>
@@ -821,7 +836,7 @@
         <v>6.2998558385391634</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>338.15</v>
       </c>
@@ -853,7 +868,7 @@
         <v>4.8506571087216246</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>343.15</v>
       </c>
@@ -894,13 +909,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
@@ -932,7 +947,7 @@
         <v>308.14999999999998</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>308.14999999999998</v>
       </c>
@@ -964,7 +979,7 @@
         <v>13090</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>318.14999999999998</v>
       </c>
@@ -996,7 +1011,7 @@
         <v>12640</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>328.15</v>
       </c>
@@ -1028,7 +1043,7 @@
         <v>13110</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>338.15</v>
       </c>
@@ -1060,7 +1075,7 @@
         <v>12180</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>343.15</v>
       </c>
@@ -1090,6 +1105,661 @@
       </c>
       <c r="J6">
         <v>12590</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>253.15</v>
+      </c>
+      <c r="C1">
+        <v>258.14999999999998</v>
+      </c>
+      <c r="D1">
+        <v>266.14999999999998</v>
+      </c>
+      <c r="E1">
+        <v>275.14999999999998</v>
+      </c>
+      <c r="F1">
+        <v>280.14999999999998</v>
+      </c>
+      <c r="G1">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="H1">
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I1">
+        <v>303.14999999999998</v>
+      </c>
+      <c r="J1">
+        <v>308.14999999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>308.14999999999998</v>
+      </c>
+      <c r="B2">
+        <v>4490</v>
+      </c>
+      <c r="C2">
+        <v>5170</v>
+      </c>
+      <c r="D2">
+        <v>6470</v>
+      </c>
+      <c r="E2">
+        <v>6790</v>
+      </c>
+      <c r="F2">
+        <v>8000</v>
+      </c>
+      <c r="G2">
+        <v>10210</v>
+      </c>
+      <c r="H2">
+        <v>12330</v>
+      </c>
+      <c r="I2">
+        <v>12310</v>
+      </c>
+      <c r="J2">
+        <v>13090</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>318.14999999999998</v>
+      </c>
+      <c r="B3">
+        <v>4230</v>
+      </c>
+      <c r="C3">
+        <v>4900</v>
+      </c>
+      <c r="D3">
+        <v>6260</v>
+      </c>
+      <c r="E3">
+        <v>6780</v>
+      </c>
+      <c r="F3">
+        <v>8370</v>
+      </c>
+      <c r="G3">
+        <v>9970</v>
+      </c>
+      <c r="H3">
+        <v>11520</v>
+      </c>
+      <c r="I3">
+        <v>13040</v>
+      </c>
+      <c r="J3">
+        <v>12640</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>328.15</v>
+      </c>
+      <c r="B4">
+        <v>3780</v>
+      </c>
+      <c r="C4">
+        <v>4710</v>
+      </c>
+      <c r="D4">
+        <v>6030</v>
+      </c>
+      <c r="E4">
+        <v>6830</v>
+      </c>
+      <c r="F4">
+        <v>8380</v>
+      </c>
+      <c r="G4">
+        <v>9940</v>
+      </c>
+      <c r="H4">
+        <v>11500</v>
+      </c>
+      <c r="I4">
+        <v>13070</v>
+      </c>
+      <c r="J4">
+        <v>13110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>338.15</v>
+      </c>
+      <c r="B5">
+        <v>2600</v>
+      </c>
+      <c r="C5">
+        <v>3170</v>
+      </c>
+      <c r="D5">
+        <v>4610</v>
+      </c>
+      <c r="E5">
+        <v>6320</v>
+      </c>
+      <c r="F5">
+        <v>8140</v>
+      </c>
+      <c r="G5">
+        <v>9550</v>
+      </c>
+      <c r="H5">
+        <v>11290</v>
+      </c>
+      <c r="I5">
+        <v>12100</v>
+      </c>
+      <c r="J5">
+        <v>12180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>343.15</v>
+      </c>
+      <c r="B6">
+        <v>2300</v>
+      </c>
+      <c r="C6">
+        <v>3000</v>
+      </c>
+      <c r="D6">
+        <v>3830</v>
+      </c>
+      <c r="E6">
+        <v>5560</v>
+      </c>
+      <c r="F6">
+        <v>7600</v>
+      </c>
+      <c r="G6">
+        <v>8700</v>
+      </c>
+      <c r="H6">
+        <v>11290</v>
+      </c>
+      <c r="I6">
+        <v>12500</v>
+      </c>
+      <c r="J6">
+        <v>12590</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>253.15</v>
+      </c>
+      <c r="C13">
+        <v>258.14999999999998</v>
+      </c>
+      <c r="D13">
+        <v>266.14999999999998</v>
+      </c>
+      <c r="E13">
+        <v>275.14999999999998</v>
+      </c>
+      <c r="F13">
+        <v>280.14999999999998</v>
+      </c>
+      <c r="G13">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="H13">
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I13">
+        <v>303.14999999999998</v>
+      </c>
+      <c r="J13">
+        <v>308.14999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>308.14999999999998</v>
+      </c>
+      <c r="B14">
+        <v>2.1099624060150375</v>
+      </c>
+      <c r="C14">
+        <v>2.3100983020554064</v>
+      </c>
+      <c r="D14">
+        <v>2.7003338898163607</v>
+      </c>
+      <c r="E14">
+        <v>3.7002724795640325</v>
+      </c>
+      <c r="F14">
+        <v>4.8989589712186161</v>
+      </c>
+      <c r="G14">
+        <v>5.0897308075772685</v>
+      </c>
+      <c r="H14">
+        <v>7.1686046511627906</v>
+      </c>
+      <c r="I14">
+        <v>8.4027303754266214</v>
+      </c>
+      <c r="J14">
+        <v>8.4017971758664949</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>318.14999999999998</v>
+      </c>
+      <c r="B15">
+        <v>1.8399304045237059</v>
+      </c>
+      <c r="C15">
+        <v>2.0399666944213157</v>
+      </c>
+      <c r="D15">
+        <v>2.3703142748958728</v>
+      </c>
+      <c r="E15">
+        <v>3.1201104463874829</v>
+      </c>
+      <c r="F15">
+        <v>3.7299465240641712</v>
+      </c>
+      <c r="G15">
+        <v>4.0495532087733546</v>
+      </c>
+      <c r="H15">
+        <v>5.459715639810427</v>
+      </c>
+      <c r="I15">
+        <v>7.520184544405998</v>
+      </c>
+      <c r="J15">
+        <v>7.9797979797979801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>328.15</v>
+      </c>
+      <c r="B16">
+        <v>1.6399132321041214</v>
+      </c>
+      <c r="C16">
+        <v>1.7901938426453821</v>
+      </c>
+      <c r="D16">
+        <v>2.080027595722663</v>
+      </c>
+      <c r="E16">
+        <v>2.7396710790212597</v>
+      </c>
+      <c r="F16">
+        <v>3.1397527163731733</v>
+      </c>
+      <c r="G16">
+        <v>3.4099485420240137</v>
+      </c>
+      <c r="H16">
+        <v>4.4992175273865413</v>
+      </c>
+      <c r="I16">
+        <v>6.0397412199630311</v>
+      </c>
+      <c r="J16">
+        <v>6.2998558385391634</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>338.15</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1.5600393700787401</v>
+      </c>
+      <c r="D17">
+        <v>1.8603712671509283</v>
+      </c>
+      <c r="E17">
+        <v>2.2898550724637681</v>
+      </c>
+      <c r="F17">
+        <v>2.630048465266559</v>
+      </c>
+      <c r="G17">
+        <v>2.8296296296296295</v>
+      </c>
+      <c r="H17">
+        <v>3.6596434359805512</v>
+      </c>
+      <c r="I17">
+        <v>4.7996826656088851</v>
+      </c>
+      <c r="J17">
+        <v>4.8506571087216246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>343.15</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1.7401181281235802</v>
+      </c>
+      <c r="E18">
+        <v>2.0600222304557243</v>
+      </c>
+      <c r="F18">
+        <v>2.3802067021609772</v>
+      </c>
+      <c r="G18">
+        <v>2.5603296056503826</v>
+      </c>
+      <c r="H18">
+        <v>3.3903903903903903</v>
+      </c>
+      <c r="I18">
+        <v>4.4294826364280651</v>
+      </c>
+      <c r="J18">
+        <v>4.469293574724885</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>253.15</v>
+      </c>
+      <c r="C21">
+        <v>258.14999999999998</v>
+      </c>
+      <c r="D21">
+        <v>266.14999999999998</v>
+      </c>
+      <c r="E21">
+        <v>275.14999999999998</v>
+      </c>
+      <c r="F21">
+        <v>280.14999999999998</v>
+      </c>
+      <c r="G21">
+        <v>283.14999999999998</v>
+      </c>
+      <c r="H21">
+        <v>293.14999999999998</v>
+      </c>
+      <c r="I21">
+        <v>303.14999999999998</v>
+      </c>
+      <c r="J21">
+        <v>308.14999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>308.14999999999998</v>
+      </c>
+      <c r="B22">
+        <f>B2/B14</f>
+        <v>2128</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:L22" si="0">C2/C14</f>
+        <v>2238</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>2396</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>1835</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1633</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1720</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>1465</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>1558.0000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>318.14999999999998</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ref="B23:L27" si="1">B3/B15</f>
+        <v>2299</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>2402</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>2641</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>2173</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>2244</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>2462.0000000000005</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>2110</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>1734</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>328.15</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>2305</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>2631</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>2899</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>2493</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>2669</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>2915</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>2556</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>2164</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>338.15</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>2032.0000000000002</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>2478</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>2760</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>3095</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>3375</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>3085</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>2521</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>343.15</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>2300</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>2201</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>2699</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>3193</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>3398</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>3330</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>2822</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>2817</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f>MAX(B22:J27)</f>
+        <v>3398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>